<commit_message>
20240312 SGA BreatheAir 6.8L Green 20240308
</commit_message>
<xml_diff>
--- a/LM2ReadandList/SGAForm_1.xlsx
+++ b/LM2ReadandList/SGAForm_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ams\Original\LM2ReadandList\LM2ReadandList\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F00019\Desktop\HEJMO\LM2ReadandList 20240312\LM2ReadandList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CE53B1-774C-4CC9-9C7E-DBEAD1623268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62C006C-B1D9-4BE5-B90E-A601F58D4F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SGA_1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -357,6 +357,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -398,51 +443,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -464,9 +464,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -504,9 +504,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -539,26 +539,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -591,26 +574,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -787,122 +753,130 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="5" width="13.125" customWidth="1"/>
-    <col min="6" max="6" width="9.875" customWidth="1"/>
-    <col min="7" max="7" width="16.5" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="1" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="5" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="45" customHeight="1" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
     </row>
-    <row r="2" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="45" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="32"/>
     </row>
-    <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="45" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="35"/>
     </row>
-    <row r="4" spans="1:12" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="45" customHeight="1" thickBot="1">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="38"/>
     </row>
-    <row r="5" spans="1:12" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
+    <row r="5" spans="1:12" ht="56.1" customHeight="1" thickBot="1">
+      <c r="A5" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="28"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="21"/>
     </row>
-    <row r="6" spans="1:12" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
+    <row r="6" spans="1:12" ht="56.1" customHeight="1" thickBot="1">
+      <c r="A6" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="28"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="7"/>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:12" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+    <row r="7" spans="1:12" ht="55.5" customHeight="1" thickBot="1">
+      <c r="A7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="37"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="9"/>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:12" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+    <row r="8" spans="1:12" ht="56.1" customHeight="1" thickBot="1">
+      <c r="A8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="28"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="9"/>
       <c r="H8" s="10"/>
       <c r="L8" s="11"/>
     </row>
-    <row r="9" spans="1:12" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="s">
+    <row r="9" spans="1:12" ht="56.1" customHeight="1" thickBot="1">
+      <c r="A9" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="32"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="D2:H4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:F7"/>
@@ -910,12 +884,6 @@
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:F9"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="D2:H4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>